<commit_message>
updates after peer review
</commit_message>
<xml_diff>
--- a/data/ClinicalLinkagewithFiles_niceNames.xlsx
+++ b/data/ClinicalLinkagewithFiles_niceNames.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10414"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10714"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/4472525/Dropbox (Moffitt Cancer Center)/SARCOMA_AVATAR/github_repo/landscape_sarcomas_orien/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B640778D-5DC2-4742-9C3C-03EAD6E183F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DEEFCD88-3AD8-D24B-AE20-3C9F5D208B16}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="51200" yWindow="500" windowWidth="38400" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="12100" windowWidth="48540" windowHeight="8960" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="fusion_reassigned" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="89">
   <si>
     <t>orien_avatar_key</t>
   </si>
@@ -272,6 +272,21 @@
   </si>
   <si>
     <t>SL000005.genes.results</t>
+  </si>
+  <si>
+    <t>cdc_revision</t>
+  </si>
+  <si>
+    <t>cdc_nice_name</t>
+  </si>
+  <si>
+    <t>reviewer_remove</t>
+  </si>
+  <si>
+    <t>not_applicable_germline</t>
+  </si>
+  <si>
+    <t>Not Applicable Germline</t>
   </si>
 </sst>
 </file>
@@ -611,19 +626,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:X6"/>
+  <dimension ref="A1:AA6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="X5" sqref="X5"/>
+      <selection activeCell="AA8" sqref="AA8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="7" max="7" width="14" customWidth="1"/>
     <col min="15" max="15" width="14.5" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="31.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -696,8 +712,17 @@
       <c r="X1" t="s">
         <v>23</v>
       </c>
+      <c r="Y1" t="s">
+        <v>84</v>
+      </c>
+      <c r="Z1" t="s">
+        <v>85</v>
+      </c>
+      <c r="AA1" t="s">
+        <v>86</v>
+      </c>
     </row>
-    <row r="2" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>50</v>
       </c>
@@ -767,8 +792,17 @@
       <c r="X2" t="s">
         <v>39</v>
       </c>
+      <c r="Y2" t="s">
+        <v>87</v>
+      </c>
+      <c r="Z2" t="s">
+        <v>88</v>
+      </c>
+      <c r="AA2" t="b">
+        <v>0</v>
+      </c>
     </row>
-    <row r="3" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>50</v>
       </c>
@@ -838,8 +872,17 @@
       <c r="X3" t="s">
         <v>39</v>
       </c>
+      <c r="Y3" t="s">
+        <v>37</v>
+      </c>
+      <c r="Z3" t="s">
+        <v>39</v>
+      </c>
+      <c r="AA3" t="b">
+        <v>0</v>
+      </c>
     </row>
-    <row r="4" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>51</v>
       </c>
@@ -909,8 +952,17 @@
       <c r="X4" t="s">
         <v>39</v>
       </c>
+      <c r="Y4" t="s">
+        <v>37</v>
+      </c>
+      <c r="Z4" t="s">
+        <v>39</v>
+      </c>
+      <c r="AA4" t="b">
+        <v>0</v>
+      </c>
     </row>
-    <row r="5" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>52</v>
       </c>
@@ -980,8 +1032,17 @@
       <c r="X5" t="s">
         <v>49</v>
       </c>
+      <c r="Y5" t="s">
+        <v>87</v>
+      </c>
+      <c r="Z5" t="s">
+        <v>88</v>
+      </c>
+      <c r="AA5" t="b">
+        <v>0</v>
+      </c>
     </row>
-    <row r="6" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>53</v>
       </c>
@@ -1050,6 +1111,15 @@
       </c>
       <c r="X6" t="s">
         <v>49</v>
+      </c>
+      <c r="Y6" t="s">
+        <v>47</v>
+      </c>
+      <c r="Z6" t="s">
+        <v>49</v>
+      </c>
+      <c r="AA6" t="b">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>